<commit_message>
last update with adjustment for record tests
</commit_message>
<xml_diff>
--- a/Projeto-Casos-Teste-Equipe_Ed_Fco_Jess_vFinal.xlsx
+++ b/Projeto-Casos-Teste-Equipe_Ed_Fco_Jess_vFinal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manedsil\Downloads\09 Qaulidade de Software e Testes\TrabalhoFinal\FinalTestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2473F876-4BA5-4FD5-ADDC-3457DBAA3069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E61671-CBBF-4123-AD01-1C3B6FE9091C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +520,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -563,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -587,21 +595,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -976,7 +983,7 @@
   <dimension ref="A1:G1009"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -993,10 +1000,10 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1009,21 +1016,21 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="19.5" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="1" t="s">
@@ -1038,7 +1045,7 @@
       <c r="E7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1055,7 +1062,7 @@
       <c r="E8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="13" t="str">
+      <c r="G8" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT01 - Acessar website https://www.saucedemo.com/</v>
       </c>
@@ -1073,7 +1080,7 @@
       <c r="E9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="13" t="str">
+      <c r="G9" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT02 - Teste de login com credenciais válidas</v>
       </c>
@@ -1091,7 +1098,7 @@
       <c r="E10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="13" t="str">
+      <c r="G10" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT03 - Adição de produto 1 no carrinho</v>
       </c>
@@ -1109,7 +1116,7 @@
       <c r="E11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="13" t="str">
+      <c r="G11" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT04 - Adição de produto 2 no carrinho</v>
       </c>
@@ -1127,7 +1134,7 @@
       <c r="E12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="13" t="str">
+      <c r="G12" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT05 - Ir para carrinho verificar itens</v>
       </c>
@@ -1145,7 +1152,7 @@
       <c r="E13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="13" t="str">
+      <c r="G13" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT06 - Remove produto 1 do carrinho</v>
       </c>
@@ -1163,7 +1170,7 @@
       <c r="E14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="13" t="str">
+      <c r="G14" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT07 - Finalização da compra</v>
       </c>
@@ -1181,7 +1188,7 @@
       <c r="E15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="13" t="str">
+      <c r="G15" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT08 - Preencher dados do comprador e clicar em continue</v>
       </c>
@@ -1199,7 +1206,7 @@
       <c r="E16" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="13" t="str">
+      <c r="G16" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v>CT09 - Encerrar compra</v>
       </c>
@@ -1208,82 +1215,82 @@
       <c r="B17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>12</v>
+      <c r="C17" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="13" t="str">
+        <v>63</v>
+      </c>
+      <c r="G17" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
-        <v>CT10 - Teste de login com credenciais inválidas</v>
+        <v>CT10 - Open more tabs</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="13" t="str">
+      <c r="C18" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
-        <v>CT11 - Open more tabs</v>
+        <v>CT11 - Test Icons Social Midia</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="45">
+    <row r="19" spans="2:7">
       <c r="B19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="13" t="str">
+      <c r="C19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
-        <v>CT12 - Test Icons Social Midia</v>
+        <v>CT12 - Logout</v>
       </c>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" s="13" t="str">
+      <c r="C20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
-        <v>CT13 - Logout</v>
+        <v>CT13 - Teste de login com credenciais inválidas</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1">
       <c r="B21" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="G21" s="13" t="str">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="G21" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v xml:space="preserve">CT14 - </v>
       </c>
@@ -1295,7 +1302,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
-      <c r="G22" s="13" t="str">
+      <c r="G22" s="12" t="str">
         <f>_xlfn.CONCAT(Table_1[[#This Row],[ID]]," - ",Table_1[[#This Row],[Descrição do Teste]])</f>
         <v xml:space="preserve">CT15 - </v>
       </c>
@@ -2316,22 +2323,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:9" ht="15.75" customHeight="1">
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="4:9" ht="16.5" customHeight="1">
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="7" spans="4:9">
       <c r="D7" s="1" t="s">

</xml_diff>